<commit_message>
menambahkan data dan rules
</commit_message>
<xml_diff>
--- a/data_n_rules.xlsx
+++ b/data_n_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@DOKUMEN\KULIAH\1. Semesteran\Smt 7\2. Sistem Pakar\Project-Sistem-Pakar-Optimasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880888A1-5A3A-4EB1-83A4-BC9DB439BC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA0A91-723D-4B05-95F8-FF06B296A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="123">
   <si>
     <t>no</t>
   </si>
@@ -392,12 +392,6 @@
   </si>
   <si>
     <t>kepercayaan_pakar</t>
-  </si>
-  <si>
-    <t>keyakinan_lulus_pakar</t>
-  </si>
-  <si>
-    <t>keyakinan_tidak_lulus__pakar</t>
   </si>
   <si>
     <t>P</t>
@@ -2277,7 +2271,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2774,10 +2768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE50FE8-E1BA-42B7-99E5-DDF7F109B393}">
-  <dimension ref="A1:F1346"/>
+  <dimension ref="A1:E1346"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2786,11 +2780,10 @@
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
     <col min="3" max="3" width="7.6328125" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="28.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -2804,13 +2797,10 @@
         <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>590</v>
       </c>
@@ -2826,11 +2816,8 @@
       <c r="E2" s="8">
         <v>65</v>
       </c>
-      <c r="F2" s="8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>521</v>
       </c>
@@ -2846,11 +2833,8 @@
       <c r="E3" s="8">
         <v>78</v>
       </c>
-      <c r="F3" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>532</v>
       </c>
@@ -2866,11 +2850,8 @@
       <c r="E4" s="8">
         <v>80</v>
       </c>
-      <c r="F4" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>415</v>
       </c>
@@ -2886,11 +2867,8 @@
       <c r="E5" s="8">
         <v>78</v>
       </c>
-      <c r="F5" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>596</v>
       </c>
@@ -2906,11 +2884,8 @@
       <c r="E6" s="8">
         <v>80</v>
       </c>
-      <c r="F6" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>502</v>
       </c>
@@ -2926,11 +2901,8 @@
       <c r="E7" s="8">
         <v>80</v>
       </c>
-      <c r="F7" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>453</v>
       </c>
@@ -2946,11 +2918,8 @@
       <c r="E8" s="8">
         <v>89</v>
       </c>
-      <c r="F8" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>454</v>
       </c>
@@ -2966,11 +2935,8 @@
       <c r="E9" s="8">
         <v>86</v>
       </c>
-      <c r="F9" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>690</v>
       </c>
@@ -2986,11 +2952,8 @@
       <c r="E10" s="8">
         <v>93</v>
       </c>
-      <c r="F10" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>493</v>
       </c>
@@ -3006,11 +2969,8 @@
       <c r="E11" s="8">
         <v>90</v>
       </c>
-      <c r="F11" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>358</v>
       </c>
@@ -3026,11 +2986,8 @@
       <c r="E12" s="8">
         <v>82</v>
       </c>
-      <c r="F12" s="8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>521</v>
       </c>
@@ -3046,11 +3003,8 @@
       <c r="E13" s="8">
         <v>82</v>
       </c>
-      <c r="F13" s="8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>538</v>
       </c>
@@ -3066,11 +3020,8 @@
       <c r="E14" s="8">
         <v>90</v>
       </c>
-      <c r="F14" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>550</v>
       </c>
@@ -3086,11 +3037,8 @@
       <c r="E15" s="8">
         <v>78</v>
       </c>
-      <c r="F15" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>387</v>
       </c>
@@ -3106,11 +3054,8 @@
       <c r="E16" s="8">
         <v>65</v>
       </c>
-      <c r="F16" s="8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>540</v>
       </c>
@@ -3126,11 +3071,8 @@
       <c r="E17" s="8">
         <v>70</v>
       </c>
-      <c r="F17" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>516</v>
       </c>
@@ -3146,11 +3088,8 @@
       <c r="E18" s="8">
         <v>78</v>
       </c>
-      <c r="F18" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>563</v>
       </c>
@@ -3166,11 +3105,8 @@
       <c r="E19" s="8">
         <v>82</v>
       </c>
-      <c r="F19" s="8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <v>518</v>
       </c>
@@ -3186,11 +3122,8 @@
       <c r="E20" s="8">
         <v>88</v>
       </c>
-      <c r="F20" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
         <v>544</v>
       </c>
@@ -3206,11 +3139,8 @@
       <c r="E21" s="8">
         <v>90</v>
       </c>
-      <c r="F21" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>413</v>
       </c>
@@ -3226,11 +3156,8 @@
       <c r="E22" s="8">
         <v>90</v>
       </c>
-      <c r="F22" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
         <v>533</v>
       </c>
@@ -3246,11 +3173,8 @@
       <c r="E23" s="8">
         <v>94</v>
       </c>
-      <c r="F23" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="8">
         <v>426</v>
       </c>
@@ -3266,11 +3190,8 @@
       <c r="E24" s="8">
         <v>90</v>
       </c>
-      <c r="F24" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="8">
         <v>528</v>
       </c>
@@ -3286,11 +3207,8 @@
       <c r="E25" s="8">
         <v>90</v>
       </c>
-      <c r="F25" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <v>338</v>
       </c>
@@ -3306,11 +3224,8 @@
       <c r="E26" s="8">
         <v>88</v>
       </c>
-      <c r="F26" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="8">
         <v>388</v>
       </c>
@@ -3326,11 +3241,8 @@
       <c r="E27" s="8">
         <v>80</v>
       </c>
-      <c r="F27" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="8">
         <v>460</v>
       </c>
@@ -3346,11 +3258,8 @@
       <c r="E28" s="8">
         <v>95</v>
       </c>
-      <c r="F28" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="8">
         <v>517</v>
       </c>
@@ -3366,11 +3275,8 @@
       <c r="E29" s="8">
         <v>100</v>
       </c>
-      <c r="F29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="8">
         <v>599</v>
       </c>
@@ -3386,11 +3292,8 @@
       <c r="E30" s="8">
         <v>75</v>
       </c>
-      <c r="F30" s="8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="8">
         <v>460</v>
       </c>
@@ -3406,11 +3309,8 @@
       <c r="E31" s="8">
         <v>80</v>
       </c>
-      <c r="F31" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="8">
         <v>331</v>
       </c>
@@ -3426,11 +3326,8 @@
       <c r="E32" s="8">
         <v>75</v>
       </c>
-      <c r="F32" s="8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="8">
         <v>493</v>
       </c>
@@ -3446,11 +3343,8 @@
       <c r="E33" s="8">
         <v>95</v>
       </c>
-      <c r="F33" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="8">
         <v>354</v>
       </c>
@@ -3466,11 +3360,8 @@
       <c r="E34" s="8">
         <v>80</v>
       </c>
-      <c r="F34" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="8">
         <v>354</v>
       </c>
@@ -3486,11 +3377,8 @@
       <c r="E35" s="8">
         <v>80</v>
       </c>
-      <c r="F35" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="8">
         <v>454</v>
       </c>
@@ -3506,11 +3394,8 @@
       <c r="E36" s="8">
         <v>80</v>
       </c>
-      <c r="F36" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="8">
         <v>301</v>
       </c>
@@ -3526,11 +3411,8 @@
       <c r="E37" s="8">
         <v>90</v>
       </c>
-      <c r="F37" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="8">
         <v>369</v>
       </c>
@@ -3546,11 +3428,8 @@
       <c r="E38" s="8">
         <v>80</v>
       </c>
-      <c r="F38" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="8">
         <v>438</v>
       </c>
@@ -3566,11 +3445,8 @@
       <c r="E39" s="8">
         <v>90</v>
       </c>
-      <c r="F39" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="8">
         <v>437</v>
       </c>
@@ -3586,11 +3462,8 @@
       <c r="E40" s="8">
         <v>80</v>
       </c>
-      <c r="F40" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="8">
         <v>459</v>
       </c>
@@ -3606,11 +3479,8 @@
       <c r="E41" s="8">
         <v>100</v>
       </c>
-      <c r="F41" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="8">
         <v>459</v>
       </c>
@@ -3626,11 +3496,8 @@
       <c r="E42" s="8">
         <v>95</v>
       </c>
-      <c r="F42" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="8">
         <v>380</v>
       </c>
@@ -3646,11 +3513,8 @@
       <c r="E43" s="8">
         <v>75</v>
       </c>
-      <c r="F43" s="8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="8">
         <v>444</v>
       </c>
@@ -3666,11 +3530,8 @@
       <c r="E44" s="8">
         <v>77</v>
       </c>
-      <c r="F44" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="8">
         <v>425</v>
       </c>
@@ -3686,11 +3547,8 @@
       <c r="E45" s="8">
         <v>80</v>
       </c>
-      <c r="F45" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="8">
         <v>580</v>
       </c>
@@ -3706,11 +3564,8 @@
       <c r="E46" s="8">
         <v>95</v>
       </c>
-      <c r="F46" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="8">
         <v>488</v>
       </c>
@@ -3726,11 +3581,8 @@
       <c r="E47" s="8">
         <v>100</v>
       </c>
-      <c r="F47" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="8">
         <v>521</v>
       </c>
@@ -3746,11 +3598,8 @@
       <c r="E48" s="8">
         <v>90</v>
       </c>
-      <c r="F48" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="8">
         <v>497</v>
       </c>
@@ -3766,11 +3615,8 @@
       <c r="E49" s="8">
         <v>90</v>
       </c>
-      <c r="F49" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="8">
         <v>456</v>
       </c>
@@ -3786,11 +3632,8 @@
       <c r="E50" s="8">
         <v>80</v>
       </c>
-      <c r="F50" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="8">
         <v>476</v>
       </c>
@@ -3804,13 +3647,10 @@
         <v>0</v>
       </c>
       <c r="E51" s="8">
-        <v>5</v>
-      </c>
-      <c r="F51" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="8">
         <v>501</v>
       </c>
@@ -3824,13 +3664,10 @@
         <v>0</v>
       </c>
       <c r="E52" s="8">
-        <v>5</v>
-      </c>
-      <c r="F52" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="8">
         <v>565</v>
       </c>
@@ -3844,13 +3681,10 @@
         <v>0</v>
       </c>
       <c r="E53" s="8">
-        <v>0</v>
-      </c>
-      <c r="F53" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="8">
         <v>370</v>
       </c>
@@ -3864,13 +3698,10 @@
         <v>0</v>
       </c>
       <c r="E54" s="8">
-        <v>0</v>
-      </c>
-      <c r="F54" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="8">
         <v>431</v>
       </c>
@@ -3884,13 +3715,10 @@
         <v>0</v>
       </c>
       <c r="E55" s="8">
-        <v>10</v>
-      </c>
-      <c r="F55" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="8">
         <v>529</v>
       </c>
@@ -3904,13 +3732,10 @@
         <v>0</v>
       </c>
       <c r="E56" s="8">
-        <v>5</v>
-      </c>
-      <c r="F56" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="8">
         <v>530</v>
       </c>
@@ -3924,13 +3749,10 @@
         <v>0</v>
       </c>
       <c r="E57" s="8">
-        <v>7</v>
-      </c>
-      <c r="F57" s="8">
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="8">
         <v>470</v>
       </c>
@@ -3944,13 +3766,10 @@
         <v>0</v>
       </c>
       <c r="E58" s="8">
-        <v>7</v>
-      </c>
-      <c r="F58" s="8">
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="8">
         <v>357</v>
       </c>
@@ -3964,13 +3783,10 @@
         <v>0</v>
       </c>
       <c r="E59" s="8">
-        <v>8</v>
-      </c>
-      <c r="F59" s="8">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="8">
         <v>402</v>
       </c>
@@ -3984,13 +3800,10 @@
         <v>0</v>
       </c>
       <c r="E60" s="8">
-        <v>30</v>
-      </c>
-      <c r="F60" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="8">
         <v>558</v>
       </c>
@@ -4004,13 +3817,10 @@
         <v>0</v>
       </c>
       <c r="E61" s="8">
-        <v>10</v>
-      </c>
-      <c r="F61" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="8">
         <v>362</v>
       </c>
@@ -4024,13 +3834,10 @@
         <v>0</v>
       </c>
       <c r="E62" s="8">
-        <v>25</v>
-      </c>
-      <c r="F62" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="8">
         <v>331</v>
       </c>
@@ -4044,13 +3851,10 @@
         <v>0</v>
       </c>
       <c r="E63" s="8">
-        <v>5</v>
-      </c>
-      <c r="F63" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="8">
         <v>550</v>
       </c>
@@ -4064,13 +3868,10 @@
         <v>0</v>
       </c>
       <c r="E64" s="8">
-        <v>5</v>
-      </c>
-      <c r="F64" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="8">
         <v>364</v>
       </c>
@@ -4086,11 +3887,8 @@
       <c r="E65" s="8">
         <v>50</v>
       </c>
-      <c r="F65" s="8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="8">
         <v>584</v>
       </c>
@@ -4106,11 +3904,8 @@
       <c r="E66" s="8">
         <v>50</v>
       </c>
-      <c r="F66" s="8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="8">
         <v>324</v>
       </c>
@@ -4124,13 +3919,10 @@
         <v>0</v>
       </c>
       <c r="E67" s="8">
-        <v>15</v>
-      </c>
-      <c r="F67" s="8">
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="8">
         <v>503</v>
       </c>
@@ -4144,13 +3936,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="8">
-        <v>10</v>
-      </c>
-      <c r="F68" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="8">
         <v>300</v>
       </c>
@@ -4164,13 +3953,10 @@
         <v>0</v>
       </c>
       <c r="E69" s="8">
-        <v>10</v>
-      </c>
-      <c r="F69" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="8">
         <v>339</v>
       </c>
@@ -4184,13 +3970,10 @@
         <v>0</v>
       </c>
       <c r="E70" s="8">
-        <v>25</v>
-      </c>
-      <c r="F70" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="8">
         <v>572</v>
       </c>
@@ -4204,13 +3987,10 @@
         <v>0</v>
       </c>
       <c r="E71" s="8">
-        <v>30</v>
-      </c>
-      <c r="F71" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="8">
         <v>592</v>
       </c>
@@ -4224,13 +4004,10 @@
         <v>0</v>
       </c>
       <c r="E72" s="8">
-        <v>35</v>
-      </c>
-      <c r="F72" s="8">
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="8">
         <v>301</v>
       </c>
@@ -4244,13 +4021,10 @@
         <v>0</v>
       </c>
       <c r="E73" s="8">
-        <v>5</v>
-      </c>
-      <c r="F73" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="8">
         <v>136</v>
       </c>
@@ -4264,13 +4038,10 @@
         <v>0</v>
       </c>
       <c r="E74" s="8">
-        <v>0</v>
-      </c>
-      <c r="F74" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="8">
         <v>383</v>
       </c>
@@ -4284,13 +4055,10 @@
         <v>0</v>
       </c>
       <c r="E75" s="8">
-        <v>40</v>
-      </c>
-      <c r="F75" s="8">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="8">
         <v>574</v>
       </c>
@@ -4304,13 +4072,10 @@
         <v>0</v>
       </c>
       <c r="E76" s="8">
-        <v>25</v>
-      </c>
-      <c r="F76" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="8">
         <v>366</v>
       </c>
@@ -4324,13 +4089,10 @@
         <v>0</v>
       </c>
       <c r="E77" s="8">
-        <v>10</v>
-      </c>
-      <c r="F77" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="8">
         <v>420</v>
       </c>
@@ -4344,13 +4106,10 @@
         <v>0</v>
       </c>
       <c r="E78" s="8">
-        <v>20</v>
-      </c>
-      <c r="F78" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="8">
         <v>599</v>
       </c>
@@ -4364,13 +4123,10 @@
         <v>0</v>
       </c>
       <c r="E79" s="8">
-        <v>30</v>
-      </c>
-      <c r="F79" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="8">
         <v>551</v>
       </c>
@@ -4384,13 +4140,10 @@
         <v>0</v>
       </c>
       <c r="E80" s="8">
-        <v>12</v>
-      </c>
-      <c r="F80" s="8">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="8">
         <v>361</v>
       </c>
@@ -4404,13 +4157,10 @@
         <v>0</v>
       </c>
       <c r="E81" s="8">
-        <v>5</v>
-      </c>
-      <c r="F81" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="8">
         <v>486</v>
       </c>
@@ -4424,13 +4174,10 @@
         <v>0</v>
       </c>
       <c r="E82" s="8">
-        <v>45</v>
-      </c>
-      <c r="F82" s="8">
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="8">
         <v>356</v>
       </c>
@@ -4444,13 +4191,10 @@
         <v>0</v>
       </c>
       <c r="E83" s="8">
-        <v>10</v>
-      </c>
-      <c r="F83" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="8">
         <v>300</v>
       </c>
@@ -4464,13 +4208,10 @@
         <v>0</v>
       </c>
       <c r="E84" s="8">
-        <v>5</v>
-      </c>
-      <c r="F84" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="8">
         <v>338</v>
       </c>
@@ -4484,13 +4225,10 @@
         <v>0</v>
       </c>
       <c r="E85" s="8">
-        <v>10</v>
-      </c>
-      <c r="F85" s="8">
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="8">
         <v>343</v>
       </c>
@@ -4504,13 +4242,10 @@
         <v>0</v>
       </c>
       <c r="E86" s="8">
-        <v>2</v>
-      </c>
-      <c r="F86" s="8">
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="8">
         <v>510</v>
       </c>
@@ -4524,13 +4259,10 @@
         <v>0</v>
       </c>
       <c r="E87" s="8">
-        <v>5</v>
-      </c>
-      <c r="F87" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="8">
         <v>341</v>
       </c>
@@ -4544,13 +4276,10 @@
         <v>0</v>
       </c>
       <c r="E88" s="8">
-        <v>35</v>
-      </c>
-      <c r="F88" s="8">
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="8">
         <v>552</v>
       </c>
@@ -4564,13 +4293,10 @@
         <v>0</v>
       </c>
       <c r="E89" s="8">
-        <v>5</v>
-      </c>
-      <c r="F89" s="8">
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="8">
         <v>393</v>
       </c>
@@ -4584,13 +4310,10 @@
         <v>0</v>
       </c>
       <c r="E90" s="8">
-        <v>30</v>
-      </c>
-      <c r="F90" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="8">
         <v>109</v>
       </c>
@@ -4604,13 +4327,10 @@
         <v>0</v>
       </c>
       <c r="E91" s="8">
-        <v>35</v>
-      </c>
-      <c r="F91" s="8">
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="8">
         <v>356</v>
       </c>
@@ -4624,13 +4344,10 @@
         <v>0</v>
       </c>
       <c r="E92" s="8">
-        <v>22</v>
-      </c>
-      <c r="F92" s="8">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="8">
         <v>512</v>
       </c>
@@ -4644,13 +4361,10 @@
         <v>0</v>
       </c>
       <c r="E93" s="8">
-        <v>20</v>
-      </c>
-      <c r="F93" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="8">
         <v>303</v>
       </c>
@@ -4664,13 +4378,10 @@
         <v>0</v>
       </c>
       <c r="E94" s="8">
-        <v>30</v>
-      </c>
-      <c r="F94" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="8">
         <v>337</v>
       </c>
@@ -4684,13 +4395,10 @@
         <v>0</v>
       </c>
       <c r="E95" s="8">
-        <v>45</v>
-      </c>
-      <c r="F95" s="8">
         <v>55</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="8">
         <v>535</v>
       </c>
@@ -4704,13 +4412,10 @@
         <v>0</v>
       </c>
       <c r="E96" s="8">
-        <v>20</v>
-      </c>
-      <c r="F96" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="8">
         <v>342</v>
       </c>
@@ -4724,13 +4429,10 @@
         <v>0</v>
       </c>
       <c r="E97" s="8">
-        <v>20</v>
-      </c>
-      <c r="F97" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="8">
         <v>253</v>
       </c>
@@ -4744,13 +4446,10 @@
         <v>0</v>
       </c>
       <c r="E98" s="8">
-        <v>22</v>
-      </c>
-      <c r="F98" s="8">
         <v>78</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="8">
         <v>458</v>
       </c>
@@ -4764,13 +4463,10 @@
         <v>0</v>
       </c>
       <c r="E99" s="8">
-        <v>20</v>
-      </c>
-      <c r="F99" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="8">
         <v>495</v>
       </c>
@@ -4784,13 +4480,10 @@
         <v>0</v>
       </c>
       <c r="E100" s="8">
-        <v>20</v>
-      </c>
-      <c r="F100" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="8">
         <v>205</v>
       </c>
@@ -4804,13 +4497,10 @@
         <v>0</v>
       </c>
       <c r="E101" s="8">
-        <v>35</v>
-      </c>
-      <c r="F101" s="8">
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="8">
         <v>527</v>
       </c>
@@ -4826,11 +4516,8 @@
       <c r="E102" s="8">
         <v>50</v>
       </c>
-      <c r="F102" s="8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="8">
         <v>281</v>
       </c>
@@ -4844,13 +4531,10 @@
         <v>0</v>
       </c>
       <c r="E103" s="8">
-        <v>25</v>
-      </c>
-      <c r="F103" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="8">
         <v>455</v>
       </c>
@@ -4864,13 +4548,10 @@
         <v>0</v>
       </c>
       <c r="E104" s="8">
-        <v>30</v>
-      </c>
-      <c r="F104" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="8">
         <v>376</v>
       </c>
@@ -4884,13 +4565,10 @@
         <v>0</v>
       </c>
       <c r="E105" s="8">
-        <v>25</v>
-      </c>
-      <c r="F105" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="8">
         <v>120</v>
       </c>
@@ -4904,13 +4582,10 @@
         <v>0</v>
       </c>
       <c r="E106" s="8">
-        <v>20</v>
-      </c>
-      <c r="F106" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="8">
         <v>229</v>
       </c>
@@ -4924,13 +4599,10 @@
         <v>0</v>
       </c>
       <c r="E107" s="8">
-        <v>22</v>
-      </c>
-      <c r="F107" s="8">
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="8">
         <v>110</v>
       </c>
@@ -4944,9 +4616,6 @@
         <v>0</v>
       </c>
       <c r="E108" s="8">
-        <v>20</v>
-      </c>
-      <c r="F108" s="8">
         <v>80</v>
       </c>
     </row>
@@ -5000,7 +4669,7 @@
         <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -5023,13 +4692,13 @@
         <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -5167,7 +4836,7 @@
         <v>93</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -5368,7 +5037,7 @@
         <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -8242,7 +7911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10323B2C-FB51-4DC4-9248-B79761C7992D}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
memperbaiki dan memisahkan rules dan dataset
</commit_message>
<xml_diff>
--- a/data_n_rules.xlsx
+++ b/data_n_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@DOKUMEN\KULIAH\1. Semesteran\Smt 7\2. Sistem Pakar\Project-Sistem-Pakar-Optimasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA0A91-723D-4B05-95F8-FF06B296A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7225D497-E781-4320-B894-ADCD56725270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="3" r:id="rId1"/>
@@ -2270,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E05B953-7BD7-4DFA-B4D7-B8382BE77D7E}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2770,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE50FE8-E1BA-42B7-99E5-DDF7F109B393}">
   <dimension ref="A1:E1346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>